<commit_message>
solve 10 problems , one of them are difficult
</commit_message>
<xml_diff>
--- a/刷题.xlsx
+++ b/刷题.xlsx
@@ -1031,7 +1031,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1059,13 +1059,17 @@
       <c r="B2" s="2">
         <v>45843</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2">
+        <v>45846</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="2">
+        <v>45846</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">

</xml_diff>